<commit_message>
Add module 2 themes 2-5 content
</commit_message>
<xml_diff>
--- a/apps/koryxa/frontend/public/datasets/data-analyst/module-2/theme-2/raw_profiles_messy.xlsx
+++ b/apps/koryxa/frontend/public/datasets/data-analyst/module-2/theme-2/raw_profiles_messy.xlsx
@@ -16,11 +16,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -46,6 +50,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -53,31 +62,11 @@
           <t>Export profils — KORYXA</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Date export</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2026-01-13</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t/>
+          <t>Généré le 2026-01-16 09:00:00</t>
         </is>
       </c>
     </row>
@@ -106,12 +95,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t> Togo </t>
+          <t> TOGO </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t> web</t>
+          <t>Mobile</t>
         </is>
       </c>
     </row>
@@ -123,7 +112,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BENIN</t>
+          <t>Benin</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -140,12 +129,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>  Togo</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t/>
+          <t> web</t>
         </is>
       </c>
     </row>
@@ -157,12 +146,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t> Togo</t>
+          <t>Togo </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mobile</t>
+          <t/>
         </is>
       </c>
     </row>
@@ -174,12 +163,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bénin </t>
+          <t>Bénin</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t> mobile</t>
+          <t>Web</t>
         </is>
       </c>
     </row>
@@ -191,12 +180,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Benin</t>
+          <t>TOGO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t/>
+          <t>mobile</t>
         </is>
       </c>
     </row>
@@ -213,16 +202,39 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>cellulaire</t>
+          <t>Mobile </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>u008</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t> benin</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t> web</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -234,17 +246,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cette feuille est à ignorer dans l'exercice.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Elle simule un classeur Excel réel avec des infos libres.</t>
+          <t>Feuille à ignorer (texte libre).</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>